<commit_message>
Schematic and footprint complete
</commit_message>
<xml_diff>
--- a/business/pricing.xlsx
+++ b/business/pricing.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\USBKB\business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687AADCF-6CF3-408A-9D16-A992EA05D13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539C306D-03D8-431B-B148-6EC462F04C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2985" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="10 Keyboards" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Item</t>
   </si>
@@ -50,18 +50,9 @@
     <t>Bulk Price</t>
   </si>
   <si>
-    <t>Resistor</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
-    <t>https://www.digikey.ie/en/products/detail/stackpole-electronics-inc/RMCF0201FT22R0/4439990</t>
-  </si>
-  <si>
-    <t>RMCF0201FT22R0</t>
-  </si>
-  <si>
     <t>Amount required</t>
   </si>
   <si>
@@ -80,21 +71,12 @@
     <t>Keycap</t>
   </si>
   <si>
-    <t>https://www.digikey.ie/en/products/detail/cui-devices/UJ31-CH-G2-SMT-TR/8024057</t>
-  </si>
-  <si>
-    <t>UJ31-CH-G2-SMT-TR</t>
-  </si>
-  <si>
     <t>USB Type-C</t>
   </si>
   <si>
     <t>22 ohm resistor</t>
   </si>
   <si>
-    <t>16MHz oscillator</t>
-  </si>
-  <si>
     <t>Bronze switch</t>
   </si>
   <si>
@@ -107,15 +89,9 @@
     <t>https://www.aliexpress.com/item/1005004281845148.html</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Maybe this isn't needed</t>
-  </si>
-  <si>
     <t>PCB</t>
   </si>
   <si>
@@ -126,6 +102,66 @@
   </si>
   <si>
     <t>https://cart.jlcpcb.com/quote?orderType=1&amp;stencilLayer=2&amp;stencilWidth=310&amp;stencilLength=100&amp;stencilCounts=10</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ie/en/products/detail/abracon-llc/ABM8G-16-000MHZ-18-D2Y-T/2218013</t>
+  </si>
+  <si>
+    <t>ABM8G-16.000MHZ-18-D2Y-T</t>
+  </si>
+  <si>
+    <t>Kailh hotswap socket</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/4000019410050.html</t>
+  </si>
+  <si>
+    <t>16MHz crystal oscillator</t>
+  </si>
+  <si>
+    <t>Red switch</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005003981373212.html</t>
+  </si>
+  <si>
+    <t>RC0805FR-0722KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ie/en/products/detail/stackpole-electronics-inc/RMCF0805JT22R0/1757897</t>
+  </si>
+  <si>
+    <t>22pF capacitor</t>
+  </si>
+  <si>
+    <t>1uF capacitor</t>
+  </si>
+  <si>
+    <t>CC0805JRNPO9BN220</t>
+  </si>
+  <si>
+    <t>CC0805KKX7R7BB105</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ie/en/products/detail/yageo/CC0805JRNPO9BN220/302837</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ie/en/products/detail/yageo/CC0805KKX7R7BB105/2103103</t>
+  </si>
+  <si>
+    <t>Aluminium plate</t>
+  </si>
+  <si>
+    <t>Plastic case</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ie/en/products/detail/gct/USB4105-GF-A/11198441</t>
+  </si>
+  <si>
+    <t>USB4105-GF-A</t>
   </si>
 </sst>
 </file>
@@ -176,9 +212,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -202,8 +239,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A5B2A507-846B-4C1E-857D-6A1DC9B94F2A}" name="Table1" displayName="Table1" ref="A1:H19" totalsRowCount="1">
-  <autoFilter ref="A1:H18" xr:uid="{A5B2A507-846B-4C1E-857D-6A1DC9B94F2A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A5B2A507-846B-4C1E-857D-6A1DC9B94F2A}" name="Table1" displayName="Table1" ref="A1:H15" totalsRowCount="1">
+  <autoFilter ref="A1:H14" xr:uid="{A5B2A507-846B-4C1E-857D-6A1DC9B94F2A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H14">
+    <sortCondition descending="1" ref="F1:F14"/>
+  </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{FC55CD13-AEA3-4A34-8C30-C21DDC109ED5}" name="Item" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{F78DCBEF-EFE2-4614-96AB-F9F26F0F356B}" name="Item Code"/>
@@ -213,7 +253,7 @@
     <tableColumn id="5" xr3:uid="{A2756D08-6B39-4087-850F-D368262F3916}" name="Price per product" totalsRowFunction="sum" dataDxfId="0">
       <calculatedColumnFormula>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BE90050D-FF28-4B34-9EF1-38D899405D92}" name="Link" totalsRowFunction="sum"/>
+    <tableColumn id="6" xr3:uid="{BE90050D-FF28-4B34-9EF1-38D899405D92}" name="Link"/>
     <tableColumn id="8" xr3:uid="{BB457E6F-2E65-4946-B94F-0519D58C2E65}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -483,15 +523,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
@@ -515,48 +555,45 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>770</v>
       </c>
       <c r="D2">
-        <v>0.23</v>
+        <v>125.11</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="F2">
         <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>4.5999999999999999E-2</v>
+        <v>11.048675324675324</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -572,39 +609,33 @@
         <v>5.46</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C4">
-        <v>680</v>
+        <v>1000</v>
       </c>
       <c r="D4">
-        <v>196</v>
+        <v>75.91</v>
       </c>
       <c r="E4">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F4">
         <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>17.294117647058822</v>
+        <v>5.16188</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -620,145 +651,175 @@
         <v>2.67</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
       <c r="D6">
-        <v>19.690000000000001</v>
+        <v>25.91</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
         <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>1.9690000000000001</v>
+        <v>2.5910000000000002</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>35.423999999999999</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>0</v>
+        <v>1.1808000000000001</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>6.64</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
         <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>25</v>
+        <v>0.66399999999999992</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
       <c r="C9">
         <v>10</v>
       </c>
       <c r="D9">
-        <v>25.91</v>
+        <v>3.67</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9">
         <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>2.5910000000000002</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
       </c>
       <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>1.34</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>0.99</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>0.34</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D10">
-        <v>35.423999999999999</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>1.1808000000000001</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
       <c r="C13">
         <v>1</v>
       </c>
@@ -766,14 +827,21 @@
         <v>0</v>
       </c>
       <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
         <v>0</v>
       </c>
-      <c r="F13">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>0</v>
+      <c r="G13" s="1"/>
+      <c r="H13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
       <c r="C14">
         <v>1</v>
       </c>
@@ -781,105 +849,74 @@
         <v>0</v>
       </c>
       <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
         <v>0</v>
       </c>
-      <c r="F14">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>0</v>
+      <c r="G14" s="1"/>
+      <c r="H14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <v>1</v>
+      <c r="A15" t="s">
+        <v>9</v>
       </c>
       <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
+        <f>SUBTOTAL(109,Table1[Bulk Price])</f>
+        <v>332.60399999999998</v>
       </c>
       <c r="F15">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19">
-        <f>SUBTOTAL(109,Table1[Bulk Price])</f>
-        <v>334.524</v>
-      </c>
-      <c r="F19">
         <f>SUBTOTAL(109,Table1[Price per product])</f>
-        <v>31.210917647058825</v>
-      </c>
-      <c r="G19">
-        <f>SUBTOTAL(109,Table1[Link])</f>
-        <v>0</v>
+        <v>29.410355324675326</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>680</v>
+      </c>
+      <c r="D22">
+        <v>196</v>
+      </c>
+      <c r="E22">
+        <v>68</v>
+      </c>
+      <c r="F22" t="e">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{EA18C8B1-3DAC-4417-9FEF-8F55A51A578C}"/>
-    <hyperlink ref="G6" r:id="rId2" xr:uid="{6C5E3078-8309-4964-8A5F-AD228C1ACA71}"/>
-    <hyperlink ref="G3" r:id="rId3" xr:uid="{87CADB05-70DA-4477-979A-5E1D6F664E29}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{01DF3CB9-12DD-45B2-9A9E-F3EE4FEB1113}"/>
-    <hyperlink ref="G5" r:id="rId5" xr:uid="{EC767F74-82FC-4314-BC60-145D2B2C7A73}"/>
-    <hyperlink ref="G10" r:id="rId6" xr:uid="{36975494-8557-4D32-AD82-8E0F81F270C6}"/>
-    <hyperlink ref="G9" r:id="rId7" xr:uid="{72D62951-C1A1-4B07-A242-B0E2D08EF3D6}"/>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{87CADB05-70DA-4477-979A-5E1D6F664E29}"/>
+    <hyperlink ref="G22" r:id="rId2" xr:uid="{01DF3CB9-12DD-45B2-9A9E-F3EE4FEB1113}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{EC767F74-82FC-4314-BC60-145D2B2C7A73}"/>
+    <hyperlink ref="G7" r:id="rId4" xr:uid="{36975494-8557-4D32-AD82-8E0F81F270C6}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{72D62951-C1A1-4B07-A242-B0E2D08EF3D6}"/>
+    <hyperlink ref="G9" r:id="rId6" xr:uid="{2FADE902-C41E-4F62-814B-4CBC27CB74BF}"/>
+    <hyperlink ref="G12" r:id="rId7" xr:uid="{EBF092F7-4654-4215-BB30-5ACA4BF98616}"/>
+    <hyperlink ref="G4" r:id="rId8" xr:uid="{824C53BE-A827-4F48-A2E2-FAEA1D9288BF}"/>
+    <hyperlink ref="G2" r:id="rId9" xr:uid="{217CF86B-66F4-4978-B9C5-15E745E2F383}"/>
+    <hyperlink ref="G10" r:id="rId10" xr:uid="{DAC57D90-EE96-4138-A68F-87F2DB50DF21}"/>
+    <hyperlink ref="G11" r:id="rId11" xr:uid="{3A41249C-F5A4-4F54-85B0-1408C3755E91}"/>
+    <hyperlink ref="G8" r:id="rId12" xr:uid="{9E83D466-86BD-44A5-A4F1-D66641DB8063}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Plate and PCB completed, pricing list updated with shipping fees
</commit_message>
<xml_diff>
--- a/business/pricing.xlsx
+++ b/business/pricing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\USBKB\business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539C306D-03D8-431B-B148-6EC462F04C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF12D06-C13D-41F4-804A-4DD144E64285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2985" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10 Keyboards" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t>Item</t>
   </si>
@@ -53,12 +53,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>Amount required</t>
-  </si>
-  <si>
-    <t>Price per product</t>
-  </si>
-  <si>
     <t>Atmega32u4-mu</t>
   </si>
   <si>
@@ -162,13 +156,76 @@
   </si>
   <si>
     <t>USB4105-GF-A</t>
+  </si>
+  <si>
+    <t>Stabilisers</t>
+  </si>
+  <si>
+    <t>https://candykeys.com/product/jwk-plate-mount-stabiliser-pack</t>
+  </si>
+  <si>
+    <t>Amount Required</t>
+  </si>
+  <si>
+    <t>Price Per Product</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Shipper #</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Discount Threshold</t>
+  </si>
+  <si>
+    <t>Discount %</t>
+  </si>
+  <si>
+    <t>Final Shipping Cost</t>
+  </si>
+  <si>
+    <t>DigiKey</t>
+  </si>
+  <si>
+    <t>JLCPCB</t>
+  </si>
+  <si>
+    <t>Cost of Parts</t>
+  </si>
+  <si>
+    <t>Cost of Shipping</t>
+  </si>
+  <si>
+    <t>Packhelp</t>
+  </si>
+  <si>
+    <t>Total Items Cost</t>
+  </si>
+  <si>
+    <t>Shipping Cost</t>
+  </si>
+  <si>
+    <t>CPG151101S11</t>
+  </si>
+  <si>
+    <t>Xometry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-[$€-1809]* #,##0.00_-;\-[$€-1809]* #,##0.00_-;_-[$€-1809]* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +243,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -208,20 +272,50 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$€-1809]* #,##0.00_-;\-[$€-1809]* #,##0.00_-;_-[$€-1809]* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$€-1809]* #,##0.00_-;\-[$€-1809]* #,##0.00_-;_-[$€-1809]* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$€-1809]* #,##0.00_-;\-[$€-1809]* #,##0.00_-;_-[$€-1809]* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$€-1809]* #,##0.00_-;\-[$€-1809]* #,##0.00_-;_-[$€-1809]* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$€-1809]* #,##0.00_-;\-[$€-1809]* #,##0.00_-;_-[$€-1809]* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$€-1809]* #,##0.00_-;\-[$€-1809]* #,##0.00_-;_-[$€-1809]* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$€-1809]* #,##0.00_-;\-[$€-1809]* #,##0.00_-;_-[$€-1809]* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$€-1809]* #,##0.00_-;\-[$€-1809]* #,##0.00_-;_-[$€-1809]* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$€-1809]* #,##0.00_-;\-[$€-1809]* #,##0.00_-;_-[$€-1809]* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -239,22 +333,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A5B2A507-846B-4C1E-857D-6A1DC9B94F2A}" name="Table1" displayName="Table1" ref="A1:H15" totalsRowCount="1">
-  <autoFilter ref="A1:H14" xr:uid="{A5B2A507-846B-4C1E-857D-6A1DC9B94F2A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H14">
-    <sortCondition descending="1" ref="F1:F14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A5B2A507-846B-4C1E-857D-6A1DC9B94F2A}" name="Table1" displayName="Table1" ref="A1:I16" totalsRowCount="1">
+  <autoFilter ref="A1:I15" xr:uid="{A5B2A507-846B-4C1E-857D-6A1DC9B94F2A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I15">
+    <sortCondition descending="1" ref="F1:F15"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FC55CD13-AEA3-4A34-8C30-C21DDC109ED5}" name="Item" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{F78DCBEF-EFE2-4614-96AB-F9F26F0F356B}" name="Item Code"/>
     <tableColumn id="3" xr3:uid="{74C2F96D-B077-41FE-97D3-44F2D50D1991}" name="Bulk Amount"/>
-    <tableColumn id="4" xr3:uid="{BE58D40E-C9F3-4603-8913-8D8EDC5D2F3E}" name="Bulk Price" totalsRowFunction="sum"/>
-    <tableColumn id="7" xr3:uid="{14050057-8386-40CF-8EFF-AA4B79EC4B45}" name="Amount required"/>
-    <tableColumn id="5" xr3:uid="{A2756D08-6B39-4087-850F-D368262F3916}" name="Price per product" totalsRowFunction="sum" dataDxfId="0">
-      <calculatedColumnFormula>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{BE58D40E-C9F3-4603-8913-8D8EDC5D2F3E}" name="Bulk Price" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{14050057-8386-40CF-8EFF-AA4B79EC4B45}" name="Amount Required" totalsRowDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{A2756D08-6B39-4087-850F-D368262F3916}" name="Price Per Product" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="1">
+      <calculatedColumnFormula>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount Required]])/Table1[[#This Row],[Bulk Amount]]</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="10" xr3:uid="{EFA10657-4E6F-4746-946B-C366EB641E89}" name="Shipper #"/>
     <tableColumn id="6" xr3:uid="{BE90050D-FF28-4B34-9EF1-38D899405D92}" name="Link"/>
     <tableColumn id="8" xr3:uid="{BB457E6F-2E65-4946-B94F-0519D58C2E65}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8FE08B54-EF1B-4ED2-A73F-DBC0452C2048}" name="Table2" displayName="Table2" ref="A20:G25" totalsRowCount="1">
+  <autoFilter ref="A20:G24" xr:uid="{8FE08B54-EF1B-4ED2-A73F-DBC0452C2048}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{D814D6E7-02BA-4662-8171-E36B08AEDAFC}" name="Shipper #" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{860B23DE-DFF9-4D8E-9CD3-181A9FD87038}" name="Name"/>
+    <tableColumn id="3" xr3:uid="{E159C8E6-48A1-4634-A833-D80999A48180}" name="Shipping Cost"/>
+    <tableColumn id="4" xr3:uid="{C8C73543-E2B5-4932-83DB-BF0A32753EF8}" name="Discount Threshold" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{6F14FEB9-53F9-4CD8-B03C-98E0D999D5B0}" name="Discount %" dataCellStyle="Percent"/>
+    <tableColumn id="7" xr3:uid="{FFD1D024-2F5D-462B-84E6-5D06AB4D8B3E}" name="Total Items Cost" dataDxfId="5">
+      <calculatedColumnFormula>SUMIF(Table1[Shipper '#],  Table2[[#This Row],[Shipper '#]], Table1[Bulk Price])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{B0E68DB8-28BC-49A8-86E4-AD3CC8775D3A}" name="Final Shipping Cost" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="0">
+      <calculatedColumnFormula>IF(Table2[[#This Row],[Discount Threshold]] &lt;= Table2[[#This Row],[Total Items Cost]], Table2[[#This Row],[Shipping Cost]] *(100% - Table2[[#This Row],[Discount %]]), Table2[[#This Row],[Shipping Cost]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7B666BC8-EA6C-4259-AC78-5701EA26F788}" name="Table3" displayName="Table3" ref="A30:B35" totalsRowCount="1">
+  <autoFilter ref="A30:B34" xr:uid="{7B666BC8-EA6C-4259-AC78-5701EA26F788}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C05490DE-0DBF-4579-8E0A-0B5BEEA8F6F2}" name="Column1" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{2EB7FFE6-45DB-434A-89FC-6ADAD146844C}" name="Column2" totalsRowFunction="sum" dataDxfId="9">
+      <calculatedColumnFormula>Table1[[#Totals],[Bulk Price]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -523,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,14 +662,14 @@
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="27.28515625" customWidth="1"/>
-    <col min="7" max="7" width="106.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
+    <col min="8" max="8" width="107.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -555,368 +683,605 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>770</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>125.11</v>
       </c>
       <c r="E2">
         <v>68</v>
       </c>
-      <c r="F2">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
+      <c r="F2" s="2">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount Required]])/Table1[[#This Row],[Bulk Amount]]</f>
         <v>11.048675324675324</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>54.6</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
+      <c r="F3" s="2">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount Required]])/Table1[[#This Row],[Bulk Amount]]</f>
         <v>5.46</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
       </c>
       <c r="C4">
         <v>1000</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>75.91</v>
       </c>
       <c r="E4">
         <v>68</v>
       </c>
-      <c r="F4">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
+      <c r="F4" s="2">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount Required]])/Table1[[#This Row],[Bulk Amount]]</f>
         <v>5.16188</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>2.67</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
+      <c r="F5" s="2">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount Required]])/Table1[[#This Row],[Bulk Amount]]</f>
         <v>2.67</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>25.91</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
+      <c r="F6" s="2">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount Required]])/Table1[[#This Row],[Bulk Amount]]</f>
         <v>2.5910000000000002</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>30</v>
       </c>
-      <c r="D7">
-        <v>35.423999999999999</v>
+      <c r="D7" s="2">
+        <v>35.42</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>1.1808000000000001</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="2">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount Required]])/Table1[[#This Row],[Bulk Amount]]</f>
+        <v>1.1806666666666668</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>6.64</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
+      <c r="F8" s="2">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount Required]])/Table1[[#This Row],[Bulk Amount]]</f>
         <v>0.66399999999999992</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>10</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>3.67</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
+      <c r="F9" s="2">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount Required]])/Table1[[#This Row],[Bulk Amount]]</f>
         <v>0.36699999999999999</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
       </c>
       <c r="C10">
         <v>20</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>1.34</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
-      <c r="F10">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
+      <c r="F10" s="2">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount Required]])/Table1[[#This Row],[Bulk Amount]]</f>
         <v>0.13400000000000001</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>0.99</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
+      <c r="F11" s="2">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount Required]])/Table1[[#This Row],[Bulk Amount]]</f>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12">
         <v>20</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>0.34</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
-      <c r="F12">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
+      <c r="F12" s="2">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount Required]])/Table1[[#This Row],[Bulk Amount]]</f>
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2">
+        <v>51.4</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount Required]])/Table1[[#This Row],[Bulk Amount]]</f>
+        <v>5.14</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" t="s">
         <v>37</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="H13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
+      <c r="D14" s="2">
+        <v>0</v>
       </c>
       <c r="F14" s="2">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount Required]])/Table1[[#This Row],[Bulk Amount]]</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount Required]])/Table1[[#This Row],[Bulk Amount]]</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="2">
         <f>SUBTOTAL(109,Table1[Bulk Price])</f>
-        <v>332.60399999999998</v>
-      </c>
-      <c r="F15">
-        <f>SUBTOTAL(109,Table1[Price per product])</f>
-        <v>29.410355324675326</v>
+        <v>384</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2">
+        <f>SUBTOTAL(109,Table1[Price Per Product])</f>
+        <v>34.550221991341992</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="2">
+        <v>18</v>
+      </c>
+      <c r="D21" s="2">
+        <v>50</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
+        <f>SUMIF(Table1[Shipper '#],  Table2[[#This Row],[Shipper '#]], Table1[Bulk Price])</f>
+        <v>67.58</v>
+      </c>
+      <c r="G21" s="2">
+        <f>IF(Table2[[#This Row],[Discount Threshold]] &lt;= Table2[[#This Row],[Total Items Cost]], Table2[[#This Row],[Shipping Cost]] *(100% - Table2[[#This Row],[Discount %]]), Table2[[#This Row],[Shipping Cost]])</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="2">
+        <v>21</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <f>SUMIF(Table1[Shipper '#],  Table2[[#This Row],[Shipper '#]], Table1[Bulk Price])</f>
+        <v>25.91</v>
+      </c>
+      <c r="G22" s="2">
+        <f>IF(Table2[[#This Row],[Discount Threshold]] &lt;= Table2[[#This Row],[Total Items Cost]], Table2[[#This Row],[Shipping Cost]] *(100% - Table2[[#This Row],[Discount %]]), Table2[[#This Row],[Shipping Cost]])</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="2">
+        <v>6.15</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <f>SUMIF(Table1[Shipper '#],  Table2[[#This Row],[Shipper '#]], Table1[Bulk Price])</f>
+        <v>35.42</v>
+      </c>
+      <c r="G23" s="2">
+        <f>IF(Table2[[#This Row],[Discount Threshold]] &lt;= Table2[[#This Row],[Total Items Cost]], Table2[[#This Row],[Shipping Cost]] *(100% - Table2[[#This Row],[Discount %]]), Table2[[#This Row],[Shipping Cost]])</f>
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="2">
+        <v>23</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="2">
+        <f>SUMIF(Table1[Shipper '#],  Table2[[#This Row],[Shipper '#]], Table1[Bulk Price])</f>
+        <v>51.4</v>
+      </c>
+      <c r="G24" s="2">
+        <f>IF(Table2[[#This Row],[Discount Threshold]] &lt;= Table2[[#This Row],[Total Items Cost]], Table2[[#This Row],[Shipping Cost]] *(100% - Table2[[#This Row],[Discount %]]), Table2[[#This Row],[Shipping Cost]])</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="2">
+        <f>SUBTOTAL(109,Table2[Final Shipping Cost])</f>
+        <v>50.15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31">
+        <f>Table1[[#Totals],[Bulk Price]]</f>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32">
+        <f>Table2[[#Totals],[Final Shipping Cost]]</f>
+        <v>50.15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35">
+        <f>SUBTOTAL(109,Table3[Column2])</f>
+        <v>434.15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>680</v>
+      </c>
+      <c r="D38">
+        <v>196</v>
+      </c>
+      <c r="E38">
+        <v>68</v>
+      </c>
+      <c r="F38" t="e">
+        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount Required]])/Table1[[#This Row],[Bulk Amount]]</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" t="s">
         <v>13</v>
-      </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22">
-        <v>680</v>
-      </c>
-      <c r="D22">
-        <v>196</v>
-      </c>
-      <c r="E22">
-        <v>68</v>
-      </c>
-      <c r="F22" t="e">
-        <f>(Table1[[#This Row],[Bulk Price]] * Table1[[#This Row],[Amount required]])/Table1[[#This Row],[Bulk Amount]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" xr:uid="{87CADB05-70DA-4477-979A-5E1D6F664E29}"/>
-    <hyperlink ref="G22" r:id="rId2" xr:uid="{01DF3CB9-12DD-45B2-9A9E-F3EE4FEB1113}"/>
-    <hyperlink ref="G5" r:id="rId3" xr:uid="{EC767F74-82FC-4314-BC60-145D2B2C7A73}"/>
-    <hyperlink ref="G7" r:id="rId4" xr:uid="{36975494-8557-4D32-AD82-8E0F81F270C6}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{72D62951-C1A1-4B07-A242-B0E2D08EF3D6}"/>
-    <hyperlink ref="G9" r:id="rId6" xr:uid="{2FADE902-C41E-4F62-814B-4CBC27CB74BF}"/>
-    <hyperlink ref="G12" r:id="rId7" xr:uid="{EBF092F7-4654-4215-BB30-5ACA4BF98616}"/>
-    <hyperlink ref="G4" r:id="rId8" xr:uid="{824C53BE-A827-4F48-A2E2-FAEA1D9288BF}"/>
-    <hyperlink ref="G2" r:id="rId9" xr:uid="{217CF86B-66F4-4978-B9C5-15E745E2F383}"/>
-    <hyperlink ref="G10" r:id="rId10" xr:uid="{DAC57D90-EE96-4138-A68F-87F2DB50DF21}"/>
-    <hyperlink ref="G11" r:id="rId11" xr:uid="{3A41249C-F5A4-4F54-85B0-1408C3755E91}"/>
-    <hyperlink ref="G8" r:id="rId12" xr:uid="{9E83D466-86BD-44A5-A4F1-D66641DB8063}"/>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{87CADB05-70DA-4477-979A-5E1D6F664E29}"/>
+    <hyperlink ref="G37" r:id="rId2" xr:uid="{01DF3CB9-12DD-45B2-9A9E-F3EE4FEB1113}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{EC767F74-82FC-4314-BC60-145D2B2C7A73}"/>
+    <hyperlink ref="H7" r:id="rId4" xr:uid="{36975494-8557-4D32-AD82-8E0F81F270C6}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{72D62951-C1A1-4B07-A242-B0E2D08EF3D6}"/>
+    <hyperlink ref="H9" r:id="rId6" xr:uid="{2FADE902-C41E-4F62-814B-4CBC27CB74BF}"/>
+    <hyperlink ref="H12" r:id="rId7" xr:uid="{EBF092F7-4654-4215-BB30-5ACA4BF98616}"/>
+    <hyperlink ref="H4" r:id="rId8" xr:uid="{824C53BE-A827-4F48-A2E2-FAEA1D9288BF}"/>
+    <hyperlink ref="H2" r:id="rId9" xr:uid="{217CF86B-66F4-4978-B9C5-15E745E2F383}"/>
+    <hyperlink ref="H10" r:id="rId10" xr:uid="{DAC57D90-EE96-4138-A68F-87F2DB50DF21}"/>
+    <hyperlink ref="H11" r:id="rId11" xr:uid="{3A41249C-F5A4-4F54-85B0-1408C3755E91}"/>
+    <hyperlink ref="H8" r:id="rId12" xr:uid="{9E83D466-86BD-44A5-A4F1-D66641DB8063}"/>
+    <hyperlink ref="H15" r:id="rId13" xr:uid="{397927BB-1D35-464D-AE8E-FDBD21308BF7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
-  <tableParts count="1">
-    <tablePart r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <tableParts count="3">
+    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>